<commit_message>
add DNA data and relabel nadp sheet
</commit_message>
<xml_diff>
--- a/data-raw/nadp/nadp_2023-01-06.xlsx
+++ b/data-raw/nadp/nadp_2023-01-06.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Dropbox (Partners HealthCare)/_data/Copeland.2023.hypoxia.flux/data-raw/nadp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BB96FD-01F7-4B45-A85A-5A46331F2507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C53D275-FC6C-8044-9497-DB160F7BF64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12140" yWindow="2320" windowWidth="27640" windowHeight="16940" xr2:uid="{EDBF2FAC-12B1-6349-9AE1-BAB3096C537D}"/>
+    <workbookView xWindow="660" yWindow="600" windowWidth="27640" windowHeight="16940" xr2:uid="{EDBF2FAC-12B1-6349-9AE1-BAB3096C537D}"/>
   </bookViews>
   <sheets>
-    <sheet name="nad" sheetId="1" r:id="rId1"/>
+    <sheet name="nadp" sheetId="1" r:id="rId1"/>
     <sheet name="dna" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -426,7 +426,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1018,7 +1018,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:H25"/>
+      <selection activeCell="F2" sqref="F2:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1056,47 +1056,119 @@
       <c r="E2">
         <v>0</v>
       </c>
+      <c r="F2">
+        <v>45479</v>
+      </c>
+      <c r="G2">
+        <v>47505</v>
+      </c>
+      <c r="H2">
+        <v>47532</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E3">
         <f t="shared" ref="E3:E7" si="0">E4/2</f>
         <v>1.5625</v>
       </c>
+      <c r="F3">
+        <v>594246</v>
+      </c>
+      <c r="G3">
+        <v>592748</v>
+      </c>
+      <c r="H3">
+        <v>607592</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E4">
         <f t="shared" si="0"/>
         <v>3.125</v>
       </c>
+      <c r="F4">
+        <v>1094433</v>
+      </c>
+      <c r="G4">
+        <v>1084946</v>
+      </c>
+      <c r="H4">
+        <v>1085169</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E5">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
+      <c r="F5">
+        <v>2116238</v>
+      </c>
+      <c r="G5">
+        <v>2083453</v>
+      </c>
+      <c r="H5">
+        <v>2167345</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E6">
         <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
+      <c r="F6">
+        <v>3969176</v>
+      </c>
+      <c r="G6">
+        <v>4062854</v>
+      </c>
+      <c r="H6">
+        <v>4039748</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E7">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
+      <c r="F7">
+        <v>7683769</v>
+      </c>
+      <c r="G7">
+        <v>7525415</v>
+      </c>
+      <c r="H7">
+        <v>7405485</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E8">
         <f>E9/2</f>
         <v>50</v>
       </c>
+      <c r="F8">
+        <v>14950687</v>
+      </c>
+      <c r="G8">
+        <v>15095009</v>
+      </c>
+      <c r="H8">
+        <v>15088696</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E9">
         <v>100</v>
       </c>
+      <c r="F9">
+        <v>32258614</v>
+      </c>
+      <c r="G9">
+        <v>31554882</v>
+      </c>
+      <c r="H9">
+        <v>32605324</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -1110,6 +1182,15 @@
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="F10">
+        <v>4396721</v>
+      </c>
+      <c r="G10">
+        <v>4417704</v>
+      </c>
+      <c r="H10">
+        <v>4267585</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1125,6 +1206,15 @@
       <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F11">
+        <v>4690542</v>
+      </c>
+      <c r="G11">
+        <v>5008814</v>
+      </c>
+      <c r="H11">
+        <v>4866435</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1139,6 +1229,15 @@
       <c r="D12" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="F12">
+        <v>4964244</v>
+      </c>
+      <c r="G12">
+        <v>4831036</v>
+      </c>
+      <c r="H12">
+        <v>4398236</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1153,6 +1252,15 @@
       <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F13">
+        <v>4226260</v>
+      </c>
+      <c r="G13">
+        <v>5223918</v>
+      </c>
+      <c r="H13">
+        <v>4708705</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1167,6 +1275,15 @@
       <c r="D14" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="F14">
+        <v>5043638</v>
+      </c>
+      <c r="G14">
+        <v>4465126</v>
+      </c>
+      <c r="H14">
+        <v>4427658</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -1181,6 +1298,15 @@
       <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F15">
+        <v>3453634</v>
+      </c>
+      <c r="G15">
+        <v>3400906</v>
+      </c>
+      <c r="H15">
+        <v>4317786</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1195,8 +1321,17 @@
       <c r="D16" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>1445231</v>
+      </c>
+      <c r="G16">
+        <v>2108782</v>
+      </c>
+      <c r="H16">
+        <v>1575609</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1209,8 +1344,17 @@
       <c r="D17" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>1208474</v>
+      </c>
+      <c r="G17">
+        <v>1701040</v>
+      </c>
+      <c r="H17">
+        <v>2090748</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1223,8 +1367,17 @@
       <c r="D18" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>1662935</v>
+      </c>
+      <c r="G18">
+        <v>1332930</v>
+      </c>
+      <c r="H18">
+        <v>1755819</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>10</v>
       </c>
@@ -1237,8 +1390,17 @@
       <c r="D19" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>1434080</v>
+      </c>
+      <c r="G19">
+        <v>2248191</v>
+      </c>
+      <c r="H19">
+        <v>1570472</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>11</v>
       </c>
@@ -1251,8 +1413,17 @@
       <c r="D20" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>2530386</v>
+      </c>
+      <c r="G20">
+        <v>2004057</v>
+      </c>
+      <c r="H20">
+        <v>2111062</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>12</v>
       </c>
@@ -1265,8 +1436,17 @@
       <c r="D21" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>2370113</v>
+      </c>
+      <c r="G21">
+        <v>1696322</v>
+      </c>
+      <c r="H21">
+        <v>2017967</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>13</v>
       </c>
@@ -1279,8 +1459,17 @@
       <c r="D22" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>1164192</v>
+      </c>
+      <c r="G22">
+        <v>1754718</v>
+      </c>
+      <c r="H22">
+        <v>1579803</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>14</v>
       </c>
@@ -1293,8 +1482,17 @@
       <c r="D23" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>1199532</v>
+      </c>
+      <c r="G23">
+        <v>1846657</v>
+      </c>
+      <c r="H23">
+        <v>1053498</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>15</v>
       </c>
@@ -1307,8 +1505,17 @@
       <c r="D24" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>839656</v>
+      </c>
+      <c r="G24">
+        <v>839903</v>
+      </c>
+      <c r="H24">
+        <v>1040993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>16</v>
       </c>
@@ -1320,6 +1527,15 @@
       </c>
       <c r="D25" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="F25">
+        <v>980032</v>
+      </c>
+      <c r="G25">
+        <v>1157112</v>
+      </c>
+      <c r="H25">
+        <v>790798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>